<commit_message>
Updated the time logs
</commit_message>
<xml_diff>
--- a/timelogs/time_logs.xlsx
+++ b/timelogs/time_logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vult-my.sharepoint.com/personal/nedas_janusauskas_mif_stud_vu_lt/Documents/3 Pusmetis/PBL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="11_9248D3AD81FF8E02EF2EE2999A3E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28100A9B-5028-9A45-A6D5-B3F203827051}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="11_9248D3AD81FF8E02EF2EE2999A3E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{502138B4-B2F0-4B18-BD4B-47FD4F337177}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nedas_J" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Week 1</t>
   </si>
@@ -45,6 +45,9 @@
     <t>Week 2</t>
   </si>
   <si>
+    <t>Week 3</t>
+  </si>
+  <si>
     <t>Week 1 (working in a group)</t>
   </si>
   <si>
@@ -55,6 +58,12 @@
   </si>
   <si>
     <t>Week 2 (total working hours)</t>
+  </si>
+  <si>
+    <t>Week 3 (working in a group)</t>
+  </si>
+  <si>
+    <t>Week 3 (total working hours)</t>
   </si>
 </sst>
 </file>
@@ -64,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,7 +116,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -419,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,12 +444,20 @@
         <v>0.17361111111111113</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.54166666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -450,15 +467,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCAF3D7-75AC-4D5B-A4BA-6C0DF3B5896A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,12 +483,20 @@
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>0.14930555555555555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.17361111111111113</v>
       </c>
     </row>
   </sheetData>
@@ -481,15 +506,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D83133-5BF0-4B81-B3C4-8ED758F5ACF4}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,12 +522,20 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>0.13541666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.25347222222222221</v>
       </c>
     </row>
   </sheetData>
@@ -512,15 +545,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923CEF60-EE42-4C46-B16B-E987EC9AEAC6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,12 +561,20 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.18402777777777779</v>
       </c>
     </row>
   </sheetData>
@@ -543,31 +584,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4035CA1-48AA-4D41-9C1D-EBE4F8897610}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="189" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <f>SUM(Nedas_J!B1, Adomas_J!B1, Aistė_G!B1, Gabrielius_D!B1) + 4 * B1</f>
@@ -575,21 +616,38 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <f>SUM(Nedas_J!B2, Adomas_J!B2, Aistė_G!B2, Gabrielius_D!B2) + 4 * B3</f>
         <v>1.0763888888888888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <f>SUM(Nedas_J!B3, Adomas_J!B3, Aistė_G!B3, Gabrielius_D!B3) + 4 * B5</f>
+        <v>1.1527777777777777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>